<commit_message>
feat: :fire: mail sender and other changes for the next version :D
</commit_message>
<xml_diff>
--- a/signatureServer/public/files/output.xlsx
+++ b/signatureServer/public/files/output.xlsx
@@ -2490,7 +2490,7 @@
       <xdr:row>339</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1333500" cy="304800"/>
+    <xdr:ext cx="1333500" cy="219075"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr descr="1565.png" id="2" name="1565.png" title="1565.png"/>
@@ -2507,7 +2507,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1333500" cy="304800"/>
+          <a:ext cx="1333500" cy="219075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>